<commit_message>
Update RMSE_plot() plotting code for stacked bar chart instead of broken axis
</commit_message>
<xml_diff>
--- a/pop_tau (by CV).xlsx
+++ b/pop_tau (by CV).xlsx
@@ -2422,7 +2422,7 @@
         <v>44</v>
       </c>
       <c r="H11">
-        <v>2.746896523895695</v>
+        <v>2.499798810810241</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2500,7 +2500,7 @@
         <v>47</v>
       </c>
       <c r="H14">
-        <v>2.674904022260796</v>
+        <v>2.706558887634363</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -2526,7 +2526,7 @@
         <v>48</v>
       </c>
       <c r="H15">
-        <v>3.150000000000006</v>
+        <v>5.74999999999998</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -2552,7 +2552,7 @@
         <v>49</v>
       </c>
       <c r="H16">
-        <v>2.293492599297754</v>
+        <v>3.400000000000056</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2578,7 +2578,7 @@
         <v>50</v>
       </c>
       <c r="H17">
-        <v>2.139150686955866</v>
+        <v>2.069002961511835</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -2604,7 +2604,7 @@
         <v>51</v>
       </c>
       <c r="H18">
-        <v>2.018181818181825</v>
+        <v>2.018181818181819</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -2630,7 +2630,7 @@
         <v>52</v>
       </c>
       <c r="H19">
-        <v>2.018181818181823</v>
+        <v>2.01818181818182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>